<commit_message>
Inputing other types of KPI's
</commit_message>
<xml_diff>
--- a/Learning KPI.xlsx
+++ b/Learning KPI.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c8525041bb7211ab/Documentos/PROJETOS/PLANILHAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio\OneDrive\Documentos\PROJETOS\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{155CFF88-44CE-466D-A389-9CEE32CC86D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{155CFF88-44CE-466D-A389-9CEE32CC86D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{18790695-A874-497E-B16A-F90C7DDDA9DF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{84CF10A0-E2D2-4513-A2B2-8CD5AA00DB26}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1" xr2:uid="{84CF10A0-E2D2-4513-A2B2-8CD5AA00DB26}"/>
   </bookViews>
   <sheets>
     <sheet name="1°KPI" sheetId="1" r:id="rId1"/>
+    <sheet name="2°KPI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
   <si>
     <t>Vendedores</t>
   </si>
@@ -81,13 +81,16 @@
   <si>
     <t>Indicadores</t>
   </si>
+  <si>
+    <t>Se</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -144,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -156,7 +159,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -168,12 +171,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF009900"/>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1148,7 +1160,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1310,6 +1321,522 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Bahnschrift Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR">
+                <a:latin typeface="Bahnschrift Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>Desempenho</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0">
+                <a:latin typeface="Bahnschrift Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t> dos Vendedores</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Bahnschrift Light" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2°KPI'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2°KPI'!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Ana</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carlos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paulo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Marcos</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Luis</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Caique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2°KPI'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>106</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DE79-4CDA-A412-7856FED62821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2°KPI'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Se</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2°KPI'!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Ana</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carlos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paulo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Marcos</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Luis</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Caique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2°KPI'!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DE79-4CDA-A412-7856FED62821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="100"/>
+        <c:axId val="610096808"/>
+        <c:axId val="610098120"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2°KPI'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indicador</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2°KPI'!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Ana</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carlos</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Paulo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Marcos</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Luis</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Caique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2°KPI'!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DE79-4CDA-A412-7856FED62821}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="610096808"/>
+        <c:axId val="610098120"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="610096808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Avignon Pro" panose="02000503040000020004" pitchFamily="2" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="610098120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="610098120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Bahnschrift" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="610096808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1390,6 +1917,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2056,6 +2623,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2512,6 +3582,7 @@
                 </a:solidFill>
                 <a:latin typeface="Avignon Pro Demi"/>
               </a:rPr>
+              <a:pPr/>
               <a:t>Abr</a:t>
             </a:fld>
             <a:endParaRPr lang="pt-BR" sz="1100"/>
@@ -2622,6 +3693,7 @@
                 </a:solidFill>
                 <a:latin typeface="Avignon Pro Demi" panose="02000703030000020004" pitchFamily="2" charset="0"/>
               </a:rPr>
+              <a:pPr/>
               <a:t>Luis</a:t>
             </a:fld>
             <a:endParaRPr lang="pt-BR" sz="1100">
@@ -2631,6 +3703,47 @@
         </xdr:txBody>
       </xdr:sp>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70313DE1-EAE4-4ABA-966A-F08846967316}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2935,8 +4048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFED0378-74CA-43B9-A815-5AF5A107EEA6}">
   <dimension ref="B3:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3453,7 +4566,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C9">
-    <cfRule type="iconSet" priority="7">
+    <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="$C$11"/>
@@ -3462,7 +4575,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D9">
-    <cfRule type="iconSet" priority="6">
+    <cfRule type="iconSet" priority="7">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="$D$11"/>
@@ -3471,7 +4584,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E9">
-    <cfRule type="iconSet" priority="5">
+    <cfRule type="iconSet" priority="6">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="$E$11"/>
@@ -3480,7 +4593,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F9">
-    <cfRule type="iconSet" priority="4">
+    <cfRule type="iconSet" priority="5">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="$F$11"/>
@@ -3489,7 +4602,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G9">
-    <cfRule type="iconSet" priority="3">
+    <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="$G$11"/>
@@ -3498,7 +4611,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H9">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="$H$11"/>
@@ -3507,11 +4620,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I9">
-    <cfRule type="iconSet" priority="1">
+    <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="$I$11"/>
         <cfvo type="num" val="$I$12"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L9">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="$M$4"/>
+        <cfvo type="num" val="$N$4"/>
       </iconSet>
     </cfRule>
   </conditionalFormatting>
@@ -3527,4 +4649,134 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019A6201-9DD1-4193-9903-F1F1B7AFA323}">
+  <dimension ref="B2:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>153</v>
+      </c>
+      <c r="D3" s="6">
+        <f>AVERAGE($C$3:$C$8)*1.5</f>
+        <v>208</v>
+      </c>
+      <c r="E3" t="e">
+        <f>IF(C3&gt;D3,C3,NA())</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>213</v>
+      </c>
+      <c r="D4" s="6">
+        <f t="shared" ref="D4:D8" si="0">AVERAGE($C$3:$C$8)*1.5</f>
+        <v>208</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E8" si="1">IF(C4&gt;D4,C4,NA())</f>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>123</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+      <c r="E5" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9">
+        <v>117</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+      <c r="E6" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>120</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+      <c r="E7" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9">
+        <v>106</v>
+      </c>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>208</v>
+      </c>
+      <c r="E8" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>